<commit_message>
Implement add body variables
</commit_message>
<xml_diff>
--- a/heat-mail-fe/src/assets/HeatMailAddTemplate.xlsx
+++ b/heat-mail-fe/src/assets/HeatMailAddTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bojandab\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privatno\Diplomska\HeatMail_FE\HeatMail_FE\heat-mail-fe\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BE06ED1-B70A-4DFB-A287-2F74FE325F79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456E27F2-7FF1-45F5-845D-322783AFAFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>month</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>mail_receiver</t>
+  </si>
+  <si>
+    <t>mail_body_variables</t>
   </si>
 </sst>
 </file>
@@ -368,19 +371,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
     <col min="5" max="5" width="29.6328125" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,8 +400,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E2" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add changes for attachments
</commit_message>
<xml_diff>
--- a/heat-mail-fe/src/assets/HeatMailAddTemplate.xlsx
+++ b/heat-mail-fe/src/assets/HeatMailAddTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Privatno\Diplomska\HeatMail_FE\HeatMail_FE\heat-mail-fe\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{456E27F2-7FF1-45F5-845D-322783AFAFDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B813B0C3-A29E-451E-9835-E44BF56F79D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>month</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>mail_body_variables</t>
+  </si>
+  <si>
+    <t>mail_attachment_title</t>
   </si>
 </sst>
 </file>
@@ -371,10 +374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -382,9 +385,10 @@
     <col min="3" max="3" width="13.81640625" customWidth="1"/>
     <col min="5" max="5" width="29.6328125" customWidth="1"/>
     <col min="6" max="6" width="18.6328125" customWidth="1"/>
+    <col min="7" max="7" width="25.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -403,8 +407,11 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="E2" s="1"/>
     </row>
   </sheetData>

</xml_diff>